<commit_message>
uploader id record added
</commit_message>
<xml_diff>
--- a/song_alter_test.xlsx
+++ b/song_alter_test.xlsx
@@ -1,102 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t>ALBIDA Powerless Mix</t>
-  </si>
-  <si>
-    <t>Broken 8cmix</t>
-  </si>
-  <si>
-    <t>broken</t>
-  </si>
-  <si>
-    <t>ヒマワリ MUZIK SERVANT Remix</t>
-  </si>
-  <si>
-    <t>凛として咲く花の如く スプーキィテルミィンミックス</t>
-  </si>
-  <si>
-    <t>MAX 300 takamatt MIN REMIX</t>
-  </si>
-  <si>
-    <t>PULSE LASER</t>
-  </si>
-  <si>
-    <t>good high school</t>
-  </si>
-  <si>
-    <t>haogaoxiao</t>
-  </si>
-  <si>
-    <t>smooooch・∀・ KN mix</t>
-  </si>
-  <si>
-    <t>Love♡sicK</t>
-  </si>
-  <si>
-    <t>It's over</t>
-  </si>
-  <si>
-    <t>ガッテンだ!! Novoiski Remix</t>
-  </si>
-  <si>
-    <t>ふしぎなくすり いっきのみっくす</t>
-  </si>
-  <si>
-    <t>Love♡Shine わんだふるmix</t>
-  </si>
-  <si>
-    <t>Evans VolteX Pf arrange</t>
-  </si>
-  <si>
-    <t>jet coaster☆girl sasakure.UK tRiCkStAr Remix</t>
-  </si>
-  <si>
-    <t>Ha･lle･lu･jah</t>
-  </si>
-  <si>
-    <t>dilemma</t>
-  </si>
-  <si>
-    <t>Iterator</t>
-  </si>
-  <si>
-    <t>「月風魔伝」龍骨鬼戦 yks Remix</t>
-  </si>
-  <si>
-    <t>SurVALI</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="0" mc:Ignorable="x14ac">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -116,28 +36,28 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none">
+      <left>
         <color rgb="FF000000"/>
       </left>
-      <right style="none">
+      <right>
         <color rgb="FF000000"/>
       </right>
-      <top style="none">
+      <top>
         <color rgb="FF000000"/>
       </top>
-      <bottom style="none">
+      <bottom>
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal style="none">
+      <diagonal>
         <color rgb="FF000000"/>
       </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,6 +132,32 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+    <author>Ricebot</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Text</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="1" shapeId="0">
+      <text>
+        <t>1193015946</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="1" shapeId="0">
+      <text>
+        <t>1193015946</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,11 +444,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" sqref="B2"/>
@@ -511,109 +458,162 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ALBIDA Powerless Mix</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>albida</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>albida8</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Broken 8cmix</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ヒマワリ MUZIK SERVANT Remix</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>凛として咲く花の如く スプーキィテルミィンミックス</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAX 300 takamatt MIN REMIX</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PULSE LASER</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>good high school</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>haogaoxiao</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>9</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>smooooch・∀・ KN mix</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>10</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Love♡sicK</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>11</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>It's over</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ガッテンだ!! Novoiski Remix</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>13</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ふしぎなくすり いっきのみっくす</t>
+        </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>14</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Love♡Shine わんだふるmix</t>
+        </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>15</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Evans VolteX Pf arrange</t>
+        </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>16</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>jet coaster☆girl sasakure.UK tRiCkStAr Remix</t>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>17</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ha･lle･lu･jah</t>
+        </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>18</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>dilemma</t>
+        </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>19</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Iterator</t>
+        </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>20</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>「月風魔伝」龍骨鬼戦 yks Remix</t>
+        </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>21</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SurVALI</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>